<commit_message>
feat: magic object rank 7 generation
</commit_message>
<xml_diff>
--- a/dd5-generator/src/files/MO7.xlsx
+++ b/dd5-generator/src/files/MO7.xlsx
@@ -47,7 +47,7 @@
     <t xml:space="preserve">21-40</t>
   </si>
   <si>
-    <t xml:space="preserve">Bâtons magiques (lancer 1d10)</t>
+    <t xml:space="preserve">Batons magiques (lancer 1d10)</t>
   </si>
   <si>
     <t xml:space="preserve">41-45</t>
@@ -77,19 +77,19 @@
     <t xml:space="preserve">65-66 </t>
   </si>
   <si>
-    <t xml:space="preserve">Bouteille de l'éfrit</t>
+    <t xml:space="preserve">Bouteille de l&amp;apos;éfrit</t>
   </si>
   <si>
     <t xml:space="preserve">67-68 </t>
   </si>
   <si>
-    <t xml:space="preserve">Cape de l'arachnide</t>
+    <t xml:space="preserve">Cape de l&amp;apos;arachnide</t>
   </si>
   <si>
     <t xml:space="preserve">69-72 </t>
   </si>
   <si>
-    <t xml:space="preserve">Cierge d'invocation</t>
+    <t xml:space="preserve">Cierge d&amp;apos;invocation</t>
   </si>
   <si>
     <t xml:space="preserve">73-74 </t>
@@ -119,13 +119,13 @@
     <t xml:space="preserve">81-85 </t>
   </si>
   <si>
-    <t xml:space="preserve">Huile d'affûtage</t>
+    <t xml:space="preserve">Huile d&amp;apos;affûtage</t>
   </si>
   <si>
     <t xml:space="preserve">86 </t>
   </si>
   <si>
-    <t xml:space="preserve">Miroir d'emprisonnement</t>
+    <t xml:space="preserve">Miroir d&amp;apos;emprisonnement</t>
   </si>
   <si>
     <t xml:space="preserve">87-89 </t>
@@ -170,7 +170,7 @@
     <t xml:space="preserve">1-2 </t>
   </si>
   <si>
-    <t xml:space="preserve">Anneau de feu d'étoiles</t>
+    <t xml:space="preserve">Anneau de feu d’étoiles</t>
   </si>
   <si>
     <t xml:space="preserve">3-4 </t>
@@ -188,25 +188,97 @@
     <t xml:space="preserve">D10</t>
   </si>
   <si>
-    <t xml:space="preserve">Bâton de combat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bâton de feu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bâton de givre</t>
+    <t xml:space="preserve">Baton de combat</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Baton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> de feu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Baton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> de givre</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">7-8 </t>
   </si>
   <si>
-    <t xml:space="preserve">Bâton de puissance</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Baton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> de puissance</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">9-10 </t>
   </si>
   <si>
-    <t xml:space="preserve">Bâton de tonnerre et de foudre</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Baton</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> de tonnerre et de foudre</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">D20</t>
@@ -215,7 +287,7 @@
     <t xml:space="preserve">1-3 </t>
   </si>
   <si>
-    <t xml:space="preserve">Manuel d'exercices physiques</t>
+    <t xml:space="preserve">Manuel d’exercices physiques</t>
   </si>
   <si>
     <t xml:space="preserve">4-6 </t>
@@ -239,7 +311,7 @@
     <t xml:space="preserve">12-14 </t>
   </si>
   <si>
-    <t xml:space="preserve">Traité d'autorité et d'influence</t>
+    <t xml:space="preserve">Traité d’autorité et d’influence</t>
   </si>
   <si>
     <t xml:space="preserve">15-17 </t>
@@ -254,7 +326,7 @@
     <t xml:space="preserve">Traité de perspicacité</t>
   </si>
   <si>
-    <t xml:space="preserve">Sceptre d'absorption</t>
+    <t xml:space="preserve">Sceptre d’absorption</t>
   </si>
   <si>
     <t xml:space="preserve">Sceptre de sécurité</t>
@@ -272,7 +344,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -324,6 +396,12 @@
       <name val="Roboto"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -401,97 +479,77 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -574,7 +632,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -583,7 +641,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="48.29"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -591,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -599,7 +657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
@@ -607,7 +665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -615,7 +673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -623,7 +681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -631,7 +689,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
@@ -639,7 +697,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -647,7 +705,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
@@ -655,7 +713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -663,7 +721,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
@@ -671,7 +729,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
         <v>22</v>
       </c>
@@ -679,7 +737,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>24</v>
       </c>
@@ -687,7 +745,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
@@ -695,7 +753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
@@ -703,7 +761,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
@@ -711,7 +769,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
         <v>32</v>
       </c>
@@ -719,7 +777,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
@@ -727,7 +785,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
@@ -735,7 +793,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
@@ -743,7 +801,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
         <v>40</v>
       </c>
@@ -751,7 +809,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
@@ -759,7 +817,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
@@ -767,12 +825,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5"/>
+    <row r="24" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9"/>
       <c r="B24" s="6"/>
     </row>
-    <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -789,53 +847,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="14.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="36.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="14.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="36.86"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+    <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -855,60 +910,60 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="15" width="23.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="38.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="23.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="38.15"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+    <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="16" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
+    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="17" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
+    <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
+    <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="17" t="s">
         <v>60</v>
       </c>
     </row>
@@ -928,86 +983,82 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="19" width="32.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="42.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="32.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="42.01"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+    <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="21" t="s">
+    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
         <v>62</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
         <v>66</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+    <row r="5" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
         <v>68</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+    <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="12" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" s="2" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
+    <row r="7" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
         <v>72</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" s="2" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="21" t="s">
+    <row r="8" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
         <v>74</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1024,55 +1075,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="19.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="41.29"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+    <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
+    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
update readme and fix error
</commit_message>
<xml_diff>
--- a/dd5-generator/src/files/MO7.xlsx
+++ b/dd5-generator/src/files/MO7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann\Documents\DEV\DnD\DD5-Generator\dd5-generator\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF10B8E-839B-4F89-9AC5-7D2A80D263FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0846B04-7351-4A15-B64E-C8D979EDA219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -139,9 +139,6 @@
     <t>Tapis volant</t>
   </si>
   <si>
-    <t xml:space="preserve">96-00 </t>
-  </si>
-  <si>
     <t>Relancer sur table 8</t>
   </si>
   <si>
@@ -338,6 +335,9 @@
   </si>
   <si>
     <t>Bouteille de l'éfrit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96-100 </t>
   </si>
 </sst>
 </file>
@@ -895,7 +895,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,26 +970,26 @@
     </row>
     <row r="9" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1037,7 +1037,7 @@
         <v>25</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1082,10 +1082,10 @@
     </row>
     <row r="23" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1116,7 +1116,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>5</v>
@@ -1124,26 +1124,26 @@
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1168,7 +1168,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>7</v>
@@ -1176,42 +1176,42 @@
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>51</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1236,7 +1236,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>9</v>
@@ -1244,58 +1244,58 @@
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1320,7 +1320,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>11</v>
@@ -1328,26 +1328,26 @@
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>